<commit_message>
tried to fix scaling to adjust to range - still not working
</commit_message>
<xml_diff>
--- a/test-files/data-samples/dahlquist_estimation_sim_2_estimation_output.xlsx
+++ b/test-files/data-samples/dahlquist_estimation_sim_2_estimation_output.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kitsuneh\Desktop\samples_of_grnmap_output_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="15120" windowHeight="10560" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="20860" windowHeight="13500" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,12 @@
     <sheet name="network_optimized_thresholds" sheetId="13" r:id="rId13"/>
     <sheet name="concentration_sigmas" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -237,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,7 +272,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -485,9 +485,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -499,9 +504,9 @@
       <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -551,7 +556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -601,7 +606,7 @@
         <v>0.19225373981231059</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -651,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -701,7 +706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -751,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -801,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -851,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -901,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -951,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1001,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1101,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>-1.2938745240691605</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1251,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1303,6 +1308,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1314,9 +1324,9 @@
       <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1366,7 +1376,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1426,7 @@
         <v>2.427902982277268</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1466,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1516,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1616,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1666,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1716,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1766,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1816,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1866,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1916,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1966,7 +1976,7 @@
         <v>1.0576675967870679</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2016,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2066,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2118,6 +2128,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2125,13 +2140,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2181,7 +2196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2231,7 +2246,7 @@
         <v>0.14679091012645842</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2281,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2331,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2381,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2431,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2481,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2531,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2581,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2631,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2681,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2731,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2781,7 +2796,7 @@
         <v>-1.5158389139937409</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2831,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2881,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2933,6 +2948,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2944,9 +2964,9 @@
       <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2996,7 +3016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3046,7 +3066,7 @@
         <v>1.0289596164688299</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3096,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3146,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3196,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3246,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3296,7 +3316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -3346,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3396,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3446,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3496,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3546,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3596,7 +3616,7 @@
         <v>0.67736641508903939</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3646,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3696,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3748,6 +3768,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3755,13 +3780,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1.0343768626086041</v>
       </c>
@@ -3808,7 +3833,7 @@
         <v>0.18702559734033511</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>0.75543011722018172</v>
       </c>
@@ -3855,7 +3880,7 @@
         <v>0.29873087578292778</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>0.62144661581545402</v>
       </c>
@@ -3904,6 +3929,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3913,9 +3943,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3925,9 +3960,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3939,9 +3979,9 @@
       <selection sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3958,7 +3998,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3975,7 +4015,7 @@
         <v>1.8042757724049552</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3992,7 +4032,7 @@
         <v>-0.80805683349751156</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4009,7 +4049,7 @@
         <v>1.4342181629644168</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4026,7 +4066,7 @@
         <v>-0.6250839043852453</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4043,7 +4083,7 @@
         <v>0.22604859732799276</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4060,7 +4100,7 @@
         <v>-0.47911673621703305</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4077,7 +4117,7 @@
         <v>1.8590991219517012</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4094,7 +4134,7 @@
         <v>-1.6797480912907794</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4111,7 +4151,7 @@
         <v>-0.11865321294717533</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4128,7 +4168,7 @@
         <v>0.35762463624018409</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -4145,7 +4185,7 @@
         <v>-0.68333371327866343</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4162,7 +4202,7 @@
         <v>-1.4145401378583937</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4179,7 +4219,7 @@
         <v>1.8543020788663611</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4196,7 +4236,7 @@
         <v>1.8035904805356207</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -4215,6 +4255,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4226,9 +4271,9 @@
       <selection sqref="A1:EF16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:136">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4638,7 +4683,7 @@
         <v>59.85</v>
       </c>
     </row>
-    <row r="2" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:136">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5048,7 +5093,7 @@
         <v>1.6162863178029911</v>
       </c>
     </row>
-    <row r="3" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:136">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5458,7 +5503,7 @@
         <v>-0.40989910575871807</v>
       </c>
     </row>
-    <row r="4" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:136">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -5868,7 +5913,7 @@
         <v>1.4012176395866494</v>
       </c>
     </row>
-    <row r="5" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:136">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6278,7 +6323,7 @@
         <v>-0.24848764160718889</v>
       </c>
     </row>
-    <row r="6" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:136">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6688,7 +6733,7 @@
         <v>0.3578751409488744</v>
       </c>
     </row>
-    <row r="7" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:136">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -7098,7 +7143,7 @@
         <v>-0.45568278941615326</v>
       </c>
     </row>
-    <row r="8" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:136">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -7508,7 +7553,7 @@
         <v>1.6407510325783858</v>
       </c>
     </row>
-    <row r="9" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:136">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -7918,7 +7963,7 @@
         <v>-1.9297919701452679</v>
       </c>
     </row>
-    <row r="10" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:136">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -8328,7 +8373,7 @@
         <v>0.78311768978953178</v>
       </c>
     </row>
-    <row r="11" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:136">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -8738,7 +8783,7 @@
         <v>0.42931578098267065</v>
       </c>
     </row>
-    <row r="12" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:136">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -9148,7 +9193,7 @@
         <v>-0.63597390278109767</v>
       </c>
     </row>
-    <row r="13" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:136">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -9558,7 +9603,7 @@
         <v>-1.1509615373942459</v>
       </c>
     </row>
-    <row r="14" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:136">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -9968,7 +10013,7 @@
         <v>1.9665550796806772</v>
       </c>
     </row>
-    <row r="15" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:136">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -10378,7 +10423,7 @@
         <v>1.9632493362270715</v>
       </c>
     </row>
-    <row r="16" spans="1:136" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:136">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -10790,6 +10835,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10801,9 +10851,9 @@
       <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10814,7 +10864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -10825,7 +10875,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -10836,7 +10886,7 @@
         <v>2.5672117798516501E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -10847,7 +10897,7 @@
         <v>1.73286795139986E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -10858,7 +10908,7 @@
         <v>1.10023361993642E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10869,7 +10919,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -10880,7 +10930,7 @@
         <v>7.7016353395549506E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -10891,7 +10941,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -10902,7 +10952,7 @@
         <v>6.9314718055994498E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -10913,7 +10963,7 @@
         <v>1.65035042990463E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -10924,7 +10974,7 @@
         <v>3.0136833937388901E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -10935,7 +10985,7 @@
         <v>5.7762265046662098E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -10946,7 +10996,7 @@
         <v>1.33297534723066E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -10957,7 +11007,7 @@
         <v>1.2602676010180801E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -10968,7 +11018,7 @@
         <v>3.0136833937388901E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -10981,6 +11031,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10992,9 +11047,9 @@
       <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11005,7 +11060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -11016,7 +11071,7 @@
         <v>1.5193534405413283</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -11027,7 +11082,7 @@
         <v>3.5164755526628837E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -11038,7 +11093,7 @@
         <v>0.10788362623897983</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -11049,7 +11104,7 @@
         <v>1.5507392331320405E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11060,7 +11115,7 @@
         <v>0.15299321142959088</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -11071,7 +11126,7 @@
         <v>0.18082685067311097</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -11082,7 +11137,7 @@
         <v>0.97455846640704002</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -11093,7 +11148,7 @@
         <v>0.23604302330771212</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -11104,7 +11159,7 @@
         <v>7.8127703627311737E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -11115,7 +11170,7 @@
         <v>8.177797565835962E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -11126,7 +11181,7 @@
         <v>0.10475142748861364</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -11137,7 +11192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -11148,7 +11203,7 @@
         <v>0.19578291919085564</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -11159,7 +11214,7 @@
         <v>0.26948587278275438</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -11172,6 +11227,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11183,9 +11243,9 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -11201,6 +11261,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11212,9 +11277,9 @@
       <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -11264,7 +11329,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11314,7 +11379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -11364,7 +11429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -11414,7 +11479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -11464,7 +11529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -11514,7 +11579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -11564,7 +11629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -11614,7 +11679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -11664,7 +11729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -11714,7 +11779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -11764,7 +11829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -11814,7 +11879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -11864,7 +11929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -11914,7 +11979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -11964,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -12016,5 +12081,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>